<commit_message>
Pragati's changes & modules
</commit_message>
<xml_diff>
--- a/Resources/Indoor.xlsx
+++ b/Resources/Indoor.xlsx
@@ -1,9 +1,9 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="19330"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20228"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E8F64ED8-96BB-4AD9-BBF3-85A991344283}" xr6:coauthVersionLast="33" xr6:coauthVersionMax="33" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D4333D3E-3F40-408E-B25C-09BB7F7D33FD}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12648" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -568,6 +568,9 @@
       </c>
     </row>
   </sheetData>
+  <sortState ref="A3:A21">
+    <sortCondition ref="A3:A21"/>
+  </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Pragati's final version 1.0
</commit_message>
<xml_diff>
--- a/Resources/Indoor.xlsx
+++ b/Resources/Indoor.xlsx
@@ -1,9 +1,9 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="19330"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20228"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E8F64ED8-96BB-4AD9-BBF3-85A991344283}" xr6:coauthVersionLast="33" xr6:coauthVersionMax="33" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D4333D3E-3F40-408E-B25C-09BB7F7D33FD}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12648" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -568,6 +568,9 @@
       </c>
     </row>
   </sheetData>
+  <sortState ref="A3:A21">
+    <sortCondition ref="A3:A21"/>
+  </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>